<commit_message>
DECAF fuzzy match companies procedure - Implemented low threshold for non-match; low < score < high returns None - Added high-low threshold tests and truth column to test data - Updated unit and integration tests; all pass - Closes #3
</commit_message>
<xml_diff>
--- a/src/tests/data/fuzzy_match_companies.xlsx
+++ b/src/tests/data/fuzzy_match_companies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1d28b3282b7dd9da/Documents/github/DECAF/src/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbh634\Documents\GitHub\DECAF\src\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E828E78C-F841-4909-8830-0DEFA0F5D7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF7B8C2-F017-4104-A296-A6D0A1C9D361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="3660" windowWidth="28245" windowHeight="16245" xr2:uid="{DD5EF959-27E9-48D7-A33D-97BF0F2DF614}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{DD5EF959-27E9-48D7-A33D-97BF0F2DF614}"/>
   </bookViews>
   <sheets>
     <sheet name="fuzzy_match_companies" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>reference_name</t>
   </si>
@@ -128,13 +128,16 @@
   </si>
   <si>
     <t>Caterpillar Inc.</t>
+  </si>
+  <si>
+    <t>thresh_expected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,13 +974,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32793D21-2818-4444-A859-B18694942498}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -987,8 +992,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -998,8 +1006,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1009,8 +1020,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1020,8 +1034,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1031,8 +1048,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1042,8 +1062,11 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1053,8 +1076,11 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1064,8 +1090,11 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1075,8 +1104,11 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1086,8 +1118,11 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1097,8 +1132,11 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1109,7 +1147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1120,7 +1158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1131,7 +1169,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1142,7 +1180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1152,8 +1190,11 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1162,6 +1203,9 @@
       </c>
       <c r="C17" t="s">
         <v>22</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>